<commit_message>
add basic updated docs
</commit_message>
<xml_diff>
--- a/docs/EECS 581 - Project 3 Timesheet.xlsx
+++ b/docs/EECS 581 - Project 3 Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15e72c0730480894/3. KU/2025-2026/1 - Fall Semester/EECS 581/Projects/Project 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{11CF0167-A999-479B-82C3-6BD3867EA56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18D006A7-5C6E-4718-8E3F-F5499A79DF14}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{11CF0167-A999-479B-82C3-6BD3867EA56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DC3E360-C9B8-453A-AC2C-D7AC90BE86FC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2F0C5FD8-9E99-4E80-8D2E-BCE62E792A95}"/>
+    <workbookView xWindow="1770" yWindow="1440" windowWidth="24450" windowHeight="14040" activeTab="5" xr2:uid="{2F0C5FD8-9E99-4E80-8D2E-BCE62E792A95}"/>
   </bookViews>
   <sheets>
     <sheet name="Aiden Burke" sheetId="9" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>Added requirements and stories</t>
+  </si>
+  <si>
+    <t>Sprint work and sending messaegs</t>
+  </si>
+  <si>
+    <t>Meeting and creating tickets</t>
+  </si>
+  <si>
+    <t>Implementing multiplayer</t>
   </si>
 </sst>
 </file>
@@ -162,6 +171,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -555,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56D7639-386D-4AD2-A826-6E21D17A1B0D}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -704,35 +717,56 @@
       <c r="A16" s="3">
         <v>45950</v>
       </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>45951</v>
       </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>45952</v>
       </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45953</v>
       </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45954</v>
       </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>45955</v>
       </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>45956</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -932,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E85CE61-8B10-4CE6-B996-3193813E772C}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1082,35 +1116,56 @@
       <c r="A16" s="3">
         <v>45950</v>
       </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>45951</v>
       </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>45952</v>
       </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45953</v>
       </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45954</v>
       </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>45955</v>
       </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>45956</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1310,8 +1365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7A4D2FE-A479-4AEB-8985-CEC38BE970E7}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1459,35 +1514,56 @@
       <c r="A16" s="3">
         <v>45950</v>
       </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>45951</v>
       </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>45952</v>
       </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45953</v>
       </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45954</v>
       </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>45955</v>
       </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>45956</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1687,8 +1763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A78E55E-D750-4EE0-8872-FD4EAA1095EC}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1714,7 +1790,7 @@
       </c>
       <c r="G1" s="5">
         <f>SUM(Table1[[#All],[Hours]])</f>
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1842,35 +1918,65 @@
       <c r="A16" s="3">
         <v>45950</v>
       </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>45951</v>
       </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>45952</v>
       </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45953</v>
       </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45954</v>
       </c>
+      <c r="B20" s="2">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>45955</v>
       </c>
+      <c r="B21" s="2">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>45956</v>
+      </c>
+      <c r="B22" s="2">
+        <v>5</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -2085,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADCAF2B4-022D-482B-9B3E-2C3BF2D5A1CF}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2234,35 +2340,56 @@
       <c r="A16" s="3">
         <v>45950</v>
       </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>45951</v>
       </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>45952</v>
       </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45953</v>
       </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45954</v>
       </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>45955</v>
       </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>45956</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -2462,8 +2589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{461B9AF1-70E5-4DEB-97CB-64DB7B3CE921}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2611,35 +2738,56 @@
       <c r="A16" s="3">
         <v>45950</v>
       </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>45951</v>
       </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>45952</v>
       </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45953</v>
       </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45954</v>
       </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>45955</v>
       </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>45956</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
update prologue comments and timesheet
</commit_message>
<xml_diff>
--- a/docs/EECS 581 - Project 3 Timesheet.xlsx
+++ b/docs/EECS 581 - Project 3 Timesheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15E72C0730480894/3. KU/2025-2026/1 - Fall Semester/EECS 581/Projects/Project 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15e72c0730480894/3. KU/2025-2026/1 - Fall Semester/EECS 581/Projects/Project 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{3ED7A869-8DAD-46F5-8110-309773D82E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3241089-CD44-429E-A083-985FF6A01FA8}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{3ED7A869-8DAD-46F5-8110-309773D82E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A86F9367-F7EA-4BD8-94F1-5279C7C16700}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{2F0C5FD8-9E99-4E80-8D2E-BCE62E792A95}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Sprint 4 release and Project due (includes video)</t>
+  </si>
+  <si>
+    <t>Fix prologue comments</t>
   </si>
 </sst>
 </file>
@@ -243,6 +246,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1946,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A78E55E-D750-4EE0-8872-FD4EAA1095EC}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1973,7 +1980,7 @@
       </c>
       <c r="G1" s="5">
         <f>SUM(Table1[[#All],[Hours]])</f>
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -2299,26 +2306,41 @@
       <c r="A37" s="3">
         <v>45971</v>
       </c>
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>45972</v>
       </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>45973</v>
       </c>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>45974</v>
       </c>
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>45975</v>
       </c>
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
@@ -2327,36 +2349,60 @@
       <c r="A42" s="3">
         <v>45976</v>
       </c>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>45977</v>
       </c>
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>45978</v>
       </c>
+      <c r="B44" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>45979</v>
       </c>
+      <c r="B45" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45980</v>
       </c>
+      <c r="B46" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>45981</v>
       </c>
+      <c r="B47" s="2">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="48" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>45982</v>
       </c>
+      <c r="B48" s="2">
+        <v>1</v>
+      </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
@@ -2365,10 +2411,16 @@
       <c r="A49" s="3">
         <v>45983</v>
       </c>
+      <c r="B49" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>45984</v>
+      </c>
+      <c r="B50" s="2">
+        <v>3</v>
       </c>
       <c r="C50" t="s">
         <v>14</v>

</xml_diff>